<commit_message>
add userid batch, statuin id, and fix
</commit_message>
<xml_diff>
--- a/fast_test.xlsx
+++ b/fast_test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -659,24 +659,24 @@
   <dimension ref="A1:O24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="8.88671875" style="1"/>
-    <col min="7" max="7" width="11.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.88671875" style="1"/>
-    <col min="9" max="9" width="22.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="8.85546875" style="1"/>
+    <col min="7" max="7" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" style="1"/>
+    <col min="9" max="9" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" style="1"/>
     <col min="11" max="11" width="36" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.109375" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.88671875" style="1"/>
+    <col min="12" max="12" width="18.140625" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>2</v>
       </c>
@@ -684,7 +684,7 @@
       <c r="C1" s="19"/>
       <c r="D1" s="20"/>
     </row>
-    <row r="2" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="21"/>
       <c r="B2" s="22"/>
       <c r="C2" s="22"/>
@@ -701,7 +701,7 @@
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
     </row>
-    <row r="3" spans="1:15" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="24"/>
       <c r="B3" s="25"/>
       <c r="C3" s="25"/>
@@ -718,7 +718,7 @@
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
     </row>
-    <row r="4" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
@@ -729,12 +729,12 @@
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
     </row>
-    <row r="5" spans="1:15" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
       <c r="G6" s="8" t="s">
         <v>0</v>
       </c>
@@ -749,12 +749,12 @@
       </c>
       <c r="L6" s="17"/>
     </row>
-    <row r="7" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G7" s="4">
         <v>0</v>
       </c>
       <c r="H7" s="14">
-        <v>25.6</v>
+        <v>1</v>
       </c>
       <c r="I7" s="5">
         <v>1</v>
@@ -766,12 +766,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
       <c r="G8" s="4">
         <v>1</v>
       </c>
       <c r="H8" s="14">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="I8" s="5">
         <v>1</v>
@@ -783,12 +783,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="G9" s="4">
-        <v>2</v>
-      </c>
-      <c r="H9" s="14"/>
-      <c r="I9" s="5"/>
+    <row r="9" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="G9" s="4"/>
+      <c r="H9" s="14">
+        <v>3</v>
+      </c>
+      <c r="I9" s="5">
+        <v>1</v>
+      </c>
       <c r="K9" s="12" t="s">
         <v>6</v>
       </c>
@@ -796,10 +798,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
       <c r="G10" s="4"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="5"/>
+      <c r="H10" s="14">
+        <v>4</v>
+      </c>
+      <c r="I10" s="5">
+        <v>1</v>
+      </c>
       <c r="K10" s="12" t="s">
         <v>8</v>
       </c>
@@ -807,10 +813,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
       <c r="G11" s="4"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="5"/>
+      <c r="H11" s="14">
+        <v>5</v>
+      </c>
+      <c r="I11" s="5">
+        <v>1</v>
+      </c>
       <c r="K11" s="12" t="s">
         <v>10</v>
       </c>
@@ -818,7 +828,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
       <c r="G12" s="4"/>
       <c r="H12" s="14"/>
       <c r="I12" s="5"/>
@@ -829,76 +839,76 @@
         <v>120</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
       <c r="G13" s="4"/>
       <c r="H13" s="14"/>
       <c r="I13" s="5"/>
       <c r="K13" s="12"/>
       <c r="L13" s="5"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
       <c r="G14" s="4"/>
       <c r="H14" s="14"/>
       <c r="I14" s="5"/>
       <c r="K14" s="12"/>
       <c r="L14" s="5"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
       <c r="G15" s="4"/>
       <c r="H15" s="14"/>
       <c r="I15" s="5"/>
       <c r="K15" s="12"/>
       <c r="L15" s="5"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
       <c r="G16" s="4"/>
       <c r="H16" s="14"/>
       <c r="I16" s="5"/>
       <c r="K16" s="12"/>
       <c r="L16" s="5"/>
     </row>
-    <row r="17" spans="7:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="7:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="G17" s="4"/>
       <c r="H17" s="14"/>
       <c r="I17" s="5"/>
       <c r="K17" s="12"/>
       <c r="L17" s="5"/>
     </row>
-    <row r="18" spans="7:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="7:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="G18" s="4"/>
       <c r="H18" s="14"/>
       <c r="I18" s="5"/>
       <c r="K18" s="12"/>
       <c r="L18" s="5"/>
     </row>
-    <row r="19" spans="7:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="7:12" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G19" s="4"/>
       <c r="H19" s="14"/>
       <c r="I19" s="5"/>
       <c r="K19" s="13"/>
       <c r="L19" s="7"/>
     </row>
-    <row r="20" spans="7:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="7:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="G20" s="4"/>
       <c r="H20" s="14"/>
       <c r="I20" s="5"/>
     </row>
-    <row r="21" spans="7:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="7:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="G21" s="4"/>
       <c r="H21" s="14"/>
       <c r="I21" s="5"/>
     </row>
-    <row r="22" spans="7:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="7:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="G22" s="4"/>
       <c r="H22" s="14"/>
       <c r="I22" s="5"/>
     </row>
-    <row r="23" spans="7:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="7:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="G23" s="4"/>
       <c r="H23" s="14"/>
       <c r="I23" s="5"/>
     </row>
-    <row r="24" spans="7:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="7:12" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G24" s="6"/>
       <c r="H24" s="16"/>
       <c r="I24" s="7"/>
@@ -919,7 +929,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -931,7 +941,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>